<commit_message>
curb cut changes as of 11-26 am
curb cut changes as of 11-26 am Test Cases.xlsx
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases.xlsx
+++ b/src/com/data/Test Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="17775" windowHeight="8835" tabRatio="152" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="23115" windowHeight="6735" tabRatio="152" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9603" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9607" uniqueCount="431">
   <si>
     <t>TCID</t>
   </si>
@@ -3597,9 +3597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EH247"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" topLeftCell="A144" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X149" sqref="X149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="12.75"/>
@@ -9657,7 +9657,7 @@
     <row r="36" spans="1:132">
       <c r="A36" s="52"/>
     </row>
-    <row r="37" spans="1:132" s="9" customFormat="1" ht="409.6">
+    <row r="37" spans="1:132" s="9" customFormat="1">
       <c r="A37" s="63" t="s">
         <v>350</v>
       </c>
@@ -10424,10 +10424,10 @@
         <v>248</v>
       </c>
     </row>
-    <row r="40" spans="1:132" ht="409.6">
+    <row r="40" spans="1:132">
       <c r="A40" s="52"/>
     </row>
-    <row r="41" spans="1:132" s="9" customFormat="1" ht="409.6">
+    <row r="41" spans="1:132" s="9" customFormat="1">
       <c r="A41" s="63" t="s">
         <v>290</v>
       </c>
@@ -11184,7 +11184,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="45" spans="1:132" s="9" customFormat="1" ht="409.6">
+    <row r="45" spans="1:132" s="9" customFormat="1">
       <c r="A45" s="43" t="s">
         <v>295</v>
       </c>
@@ -11905,7 +11905,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="49" spans="1:128" s="9" customFormat="1">
       <c r="A49" s="43" t="s">
         <v>390</v>
       </c>
@@ -12602,7 +12602,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="53" spans="1:128" s="9" customFormat="1">
       <c r="A53" s="63" t="s">
         <v>391</v>
       </c>
@@ -13267,7 +13267,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:128" s="5" customFormat="1" ht="409.6">
+    <row r="56" spans="1:128" s="5" customFormat="1">
       <c r="A56" s="12"/>
       <c r="B56" s="27"/>
       <c r="C56" s="26"/>
@@ -13337,7 +13337,7 @@
       <c r="CY56" s="4"/>
       <c r="CZ56" s="23"/>
     </row>
-    <row r="57" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="57" spans="1:128" s="9" customFormat="1">
       <c r="A57" s="63" t="s">
         <v>405</v>
       </c>
@@ -14028,7 +14028,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:128" s="5" customFormat="1" ht="409.6">
+    <row r="60" spans="1:128" s="5" customFormat="1">
       <c r="A60" s="48"/>
       <c r="B60" s="27"/>
       <c r="C60" s="26"/>
@@ -14100,7 +14100,7 @@
       <c r="CY60" s="4"/>
       <c r="CZ60" s="23"/>
     </row>
-    <row r="61" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="61" spans="1:128" s="9" customFormat="1">
       <c r="A61" s="43" t="s">
         <v>396</v>
       </c>
@@ -14798,7 +14798,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="65" spans="1:128" s="9" customFormat="1">
       <c r="A65" s="63" t="s">
         <v>395</v>
       </c>
@@ -15464,7 +15464,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="69" spans="1:128" s="25" customFormat="1" ht="409.6">
+    <row r="69" spans="1:128" s="25" customFormat="1">
       <c r="A69" s="63" t="s">
         <v>392</v>
       </c>
@@ -16182,7 +16182,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="1:128" s="5" customFormat="1" ht="409.6">
+    <row r="72" spans="1:128" s="5" customFormat="1">
       <c r="A72" s="48"/>
       <c r="B72" s="27"/>
       <c r="C72" s="26"/>
@@ -16254,7 +16254,7 @@
       <c r="CY72" s="4"/>
       <c r="CZ72" s="23"/>
     </row>
-    <row r="73" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="73" spans="1:128" s="9" customFormat="1">
       <c r="A73" s="63" t="s">
         <v>364</v>
       </c>
@@ -16813,7 +16813,7 @@
       <c r="CY75" s="4"/>
       <c r="CZ75" s="23"/>
     </row>
-    <row r="77" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="77" spans="1:128" s="9" customFormat="1">
       <c r="A77" s="63" t="s">
         <v>365</v>
       </c>
@@ -17372,10 +17372,10 @@
       <c r="CY79" s="4"/>
       <c r="CZ79" s="23"/>
     </row>
-    <row r="80" spans="1:128" ht="409.6">
+    <row r="80" spans="1:128">
       <c r="D80" s="12"/>
     </row>
-    <row r="81" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="81" spans="1:128" s="9" customFormat="1">
       <c r="A81" s="63" t="s">
         <v>369</v>
       </c>
@@ -17934,7 +17934,7 @@
       <c r="CY83" s="4"/>
       <c r="CZ83" s="23"/>
     </row>
-    <row r="85" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="85" spans="1:128" s="9" customFormat="1">
       <c r="A85" s="63" t="s">
         <v>370</v>
       </c>
@@ -18496,10 +18496,10 @@
       <c r="CY87" s="4"/>
       <c r="CZ87" s="23"/>
     </row>
-    <row r="88" spans="1:128" ht="409.6">
+    <row r="88" spans="1:128">
       <c r="D88" s="12"/>
     </row>
-    <row r="89" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="89" spans="1:128" s="9" customFormat="1">
       <c r="A89" s="63" t="s">
         <v>367</v>
       </c>
@@ -19283,7 +19283,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="93" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="93" spans="1:128" s="9" customFormat="1">
       <c r="A93" s="63" t="s">
         <v>368</v>
       </c>
@@ -20064,7 +20064,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="96" spans="1:128" s="32" customFormat="1" ht="409.6">
+    <row r="96" spans="1:128" s="32" customFormat="1">
       <c r="A96" s="29"/>
       <c r="B96" s="30"/>
       <c r="C96" s="29"/>
@@ -20168,10 +20168,10 @@
       <c r="CY96" s="31"/>
       <c r="CZ96" s="31"/>
     </row>
-    <row r="97" spans="1:128" ht="409.6">
+    <row r="97" spans="1:128">
       <c r="A97" s="52"/>
     </row>
-    <row r="98" spans="1:128" s="32" customFormat="1" ht="409.6">
+    <row r="98" spans="1:128" s="32" customFormat="1">
       <c r="A98" s="29"/>
       <c r="B98" s="30"/>
       <c r="C98" s="29"/>
@@ -20275,7 +20275,7 @@
       <c r="CY98" s="31"/>
       <c r="CZ98" s="31"/>
     </row>
-    <row r="99" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="99" spans="1:128" s="9" customFormat="1">
       <c r="A99" s="62" t="s">
         <v>298</v>
       </c>
@@ -20864,7 +20864,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="103" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="103" spans="1:128" s="9" customFormat="1">
       <c r="A103" s="62" t="s">
         <v>299</v>
       </c>
@@ -21519,7 +21519,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="107" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="107" spans="1:128" s="9" customFormat="1">
       <c r="A107" s="53" t="s">
         <v>300</v>
       </c>
@@ -22125,7 +22125,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="111" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="111" spans="1:128" s="9" customFormat="1">
       <c r="A111" s="62" t="s">
         <v>289</v>
       </c>
@@ -22905,7 +22905,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="115" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="115" spans="1:128" s="9" customFormat="1">
       <c r="A115" s="62" t="s">
         <v>287</v>
       </c>
@@ -23685,7 +23685,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="119" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="119" spans="1:128" s="9" customFormat="1">
       <c r="A119" s="62" t="s">
         <v>351</v>
       </c>
@@ -24465,7 +24465,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="123" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="123" spans="1:128" s="9" customFormat="1">
       <c r="A123" s="62" t="s">
         <v>301</v>
       </c>
@@ -25198,7 +25198,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="127" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="127" spans="1:128" s="9" customFormat="1">
       <c r="A127" s="7" t="s">
         <v>398</v>
       </c>
@@ -25846,7 +25846,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="131" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="131" spans="1:128" s="9" customFormat="1">
       <c r="A131" s="7" t="s">
         <v>399</v>
       </c>
@@ -26473,7 +26473,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="135" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="135" spans="1:128" s="9" customFormat="1">
       <c r="A135" s="7" t="s">
         <v>400</v>
       </c>
@@ -27119,7 +27119,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="139" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="139" spans="1:128" s="9" customFormat="1">
       <c r="A139" s="7" t="s">
         <v>401</v>
       </c>
@@ -27745,7 +27745,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="143" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="143" spans="1:128" s="9" customFormat="1">
       <c r="A143" s="7" t="s">
         <v>402</v>
       </c>
@@ -28203,7 +28203,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="145" spans="1:128" s="5" customFormat="1" ht="51">
+    <row r="145" spans="1:129" s="5" customFormat="1" ht="51">
       <c r="A145" s="34" t="s">
         <v>3</v>
       </c>
@@ -28391,7 +28391,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="147" spans="1:128" s="9" customFormat="1" ht="409.6">
+    <row r="147" spans="1:129" s="9" customFormat="1">
       <c r="A147" s="7" t="s">
         <v>403</v>
       </c>
@@ -28463,7 +28463,7 @@
       <c r="CY147" s="8"/>
       <c r="CZ147" s="8"/>
     </row>
-    <row r="148" spans="1:128" s="11" customFormat="1" ht="38.25">
+    <row r="148" spans="1:129" s="11" customFormat="1" ht="38.25">
       <c r="A148" s="17" t="s">
         <v>2</v>
       </c>
@@ -28507,7 +28507,7 @@
         <v>13</v>
       </c>
       <c r="O148" s="15" t="s">
-        <v>12</v>
+        <v>324</v>
       </c>
       <c r="P148" s="15" t="s">
         <v>41</v>
@@ -28848,8 +28848,11 @@
       <c r="DX148" s="6" t="s">
         <v>259</v>
       </c>
+      <c r="DY148" s="15" t="s">
+        <v>430</v>
+      </c>
     </row>
-    <row r="149" spans="1:128" s="5" customFormat="1" ht="51">
+    <row r="149" spans="1:129" s="5" customFormat="1" ht="51">
       <c r="A149" s="34" t="s">
         <v>3</v>
       </c>
@@ -28877,6 +28880,9 @@
       <c r="I149" s="5" t="s">
         <v>311</v>
       </c>
+      <c r="O149" s="5" t="s">
+        <v>323</v>
+      </c>
       <c r="R149" s="5" t="s">
         <v>394</v>
       </c>
@@ -28889,7 +28895,9 @@
       <c r="W149" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="X149" s="14"/>
+      <c r="X149" s="14" t="s">
+        <v>317</v>
+      </c>
       <c r="Y149" s="5" t="s">
         <v>14</v>
       </c>
@@ -29036,8 +29044,11 @@
       <c r="CZ149" s="24" t="s">
         <v>53</v>
       </c>
+      <c r="DY149" s="26" t="s">
+        <v>429</v>
+      </c>
     </row>
-    <row r="151" spans="1:128" s="32" customFormat="1" ht="409.6">
+    <row r="151" spans="1:129" s="32" customFormat="1">
       <c r="A151" s="29"/>
       <c r="B151" s="30"/>
       <c r="C151" s="29"/>
@@ -29141,10 +29152,10 @@
       <c r="CY151" s="31"/>
       <c r="CZ151" s="31"/>
     </row>
-    <row r="152" spans="1:128" ht="409.6">
+    <row r="152" spans="1:129">
       <c r="A152" s="52"/>
     </row>
-    <row r="153" spans="1:128" s="32" customFormat="1" ht="409.6">
+    <row r="153" spans="1:129" s="32" customFormat="1">
       <c r="A153" s="29"/>
       <c r="B153" s="30"/>
       <c r="C153" s="29"/>
@@ -29248,7 +29259,7 @@
       <c r="CY153" s="31"/>
       <c r="CZ153" s="31"/>
     </row>
-    <row r="154" spans="1:128" s="25" customFormat="1" ht="409.6">
+    <row r="154" spans="1:129" s="25" customFormat="1">
       <c r="A154" s="7" t="s">
         <v>214</v>
       </c>
@@ -29264,7 +29275,7 @@
       <c r="AY154" s="38"/>
       <c r="AZ154" s="38"/>
     </row>
-    <row r="155" spans="1:128" s="15" customFormat="1" ht="27.75" customHeight="1">
+    <row r="155" spans="1:129" s="15" customFormat="1" ht="27.75" customHeight="1">
       <c r="A155" s="17" t="s">
         <v>2</v>
       </c>
@@ -29431,7 +29442,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="156" spans="1:128" s="5" customFormat="1" ht="38.25">
+    <row r="156" spans="1:129" s="5" customFormat="1" ht="38.25">
       <c r="A156" s="33" t="s">
         <v>3</v>
       </c>
@@ -29508,7 +29519,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="157" spans="1:128" s="5" customFormat="1" ht="38.25">
+    <row r="157" spans="1:129" s="5" customFormat="1" ht="38.25">
       <c r="A157" s="33" t="s">
         <v>3</v>
       </c>
@@ -29585,7 +29596,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="158" spans="1:128" s="5" customFormat="1" ht="38.25">
+    <row r="158" spans="1:129" s="5" customFormat="1" ht="38.25">
       <c r="A158" s="33" t="s">
         <v>3</v>
       </c>
@@ -29662,7 +29673,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="159" spans="1:128" s="5" customFormat="1" ht="38.25">
+    <row r="159" spans="1:129" s="5" customFormat="1" ht="38.25">
       <c r="A159" s="33" t="s">
         <v>3</v>
       </c>
@@ -29736,7 +29747,7 @@
       <c r="AX159" s="14"/>
       <c r="AZ159" s="14"/>
     </row>
-    <row r="160" spans="1:128" s="5" customFormat="1" ht="38.25">
+    <row r="160" spans="1:129" s="5" customFormat="1" ht="38.25">
       <c r="A160" s="33" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
latest data files as of 2019-01-02
latest data files as of 2019-01-02 - Test Cases.xlsx
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases.xlsx
+++ b/src/com/data/Test Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="23115" windowHeight="6735" tabRatio="152" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="21225" windowHeight="4380" tabRatio="152" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9607" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9607" uniqueCount="433">
   <si>
     <t>TCID</t>
   </si>
@@ -1823,6 +1823,12 @@
   </si>
   <si>
     <t>filing_review_type_8085</t>
+  </si>
+  <si>
+    <t>NYCECC :: Tabular Analysis :: Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antenna ::  :: i ::  ::  :: 1000 ::  ::  ::  ::  ::  :: due :: </t>
   </si>
 </sst>
 </file>
@@ -3597,9 +3603,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EH247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X149" sqref="X149"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="12.75"/>
@@ -4768,7 +4774,7 @@
         <v>376</v>
       </c>
       <c r="X8" s="14" t="s">
-        <v>317</v>
+        <v>431</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>14</v>
@@ -16712,7 +16718,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="75" spans="1:128" s="5" customFormat="1" ht="38.25">
+    <row r="75" spans="1:128" s="5" customFormat="1" ht="51">
       <c r="A75" s="33" t="s">
         <v>3</v>
       </c>
@@ -16720,7 +16726,7 @@
         <v>272</v>
       </c>
       <c r="C75" s="25" t="s">
-        <v>366</v>
+        <v>432</v>
       </c>
       <c r="D75" s="14" t="s">
         <v>274</v>
@@ -17934,7 +17940,7 @@
       <c r="CY83" s="4"/>
       <c r="CZ83" s="23"/>
     </row>
-    <row r="85" spans="1:128" s="9" customFormat="1">
+    <row r="85" spans="1:128" s="9" customFormat="1" ht="409.6">
       <c r="A85" s="63" t="s">
         <v>370</v>
       </c>
@@ -18496,10 +18502,10 @@
       <c r="CY87" s="4"/>
       <c r="CZ87" s="23"/>
     </row>
-    <row r="88" spans="1:128">
+    <row r="88" spans="1:128" ht="409.6">
       <c r="D88" s="12"/>
     </row>
-    <row r="89" spans="1:128" s="9" customFormat="1">
+    <row r="89" spans="1:128" s="9" customFormat="1" ht="409.6">
       <c r="A89" s="63" t="s">
         <v>367</v>
       </c>
@@ -19283,7 +19289,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="93" spans="1:128" s="9" customFormat="1">
+    <row r="93" spans="1:128" s="9" customFormat="1" ht="409.6">
       <c r="A93" s="63" t="s">
         <v>368</v>
       </c>
@@ -20064,7 +20070,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="96" spans="1:128" s="32" customFormat="1">
+    <row r="96" spans="1:128" s="32" customFormat="1" ht="409.6">
       <c r="A96" s="29"/>
       <c r="B96" s="30"/>
       <c r="C96" s="29"/>
@@ -20168,10 +20174,10 @@
       <c r="CY96" s="31"/>
       <c r="CZ96" s="31"/>
     </row>
-    <row r="97" spans="1:128">
+    <row r="97" spans="1:128" ht="409.6">
       <c r="A97" s="52"/>
     </row>
-    <row r="98" spans="1:128" s="32" customFormat="1">
+    <row r="98" spans="1:128" s="32" customFormat="1" ht="409.6">
       <c r="A98" s="29"/>
       <c r="B98" s="30"/>
       <c r="C98" s="29"/>
@@ -20275,7 +20281,7 @@
       <c r="CY98" s="31"/>
       <c r="CZ98" s="31"/>
     </row>
-    <row r="99" spans="1:128" s="9" customFormat="1">
+    <row r="99" spans="1:128" s="9" customFormat="1" ht="409.6">
       <c r="A99" s="62" t="s">
         <v>298</v>
       </c>
@@ -20864,7 +20870,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="103" spans="1:128" s="9" customFormat="1">
+    <row r="103" spans="1:128" s="9" customFormat="1" ht="409.6">
       <c r="A103" s="62" t="s">
         <v>299</v>
       </c>
@@ -21519,7 +21525,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="107" spans="1:128" s="9" customFormat="1">
+    <row r="107" spans="1:128" s="9" customFormat="1" ht="409.6">
       <c r="A107" s="53" t="s">
         <v>300</v>
       </c>
@@ -22125,7 +22131,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="111" spans="1:128" s="9" customFormat="1">
+    <row r="111" spans="1:128" s="9" customFormat="1" ht="409.6">
       <c r="A111" s="62" t="s">
         <v>289</v>
       </c>
@@ -22905,7 +22911,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="115" spans="1:128" s="9" customFormat="1">
+    <row r="115" spans="1:128" s="9" customFormat="1" ht="409.6">
       <c r="A115" s="62" t="s">
         <v>287</v>
       </c>
@@ -23685,7 +23691,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="119" spans="1:128" s="9" customFormat="1">
+    <row r="119" spans="1:128" s="9" customFormat="1" ht="409.6">
       <c r="A119" s="62" t="s">
         <v>351</v>
       </c>
@@ -24465,7 +24471,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="123" spans="1:128" s="9" customFormat="1">
+    <row r="123" spans="1:128" s="9" customFormat="1" ht="409.6">
       <c r="A123" s="62" t="s">
         <v>301</v>
       </c>
@@ -25198,7 +25204,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="127" spans="1:128" s="9" customFormat="1">
+    <row r="127" spans="1:128" s="9" customFormat="1" ht="409.6">
       <c r="A127" s="7" t="s">
         <v>398</v>
       </c>
@@ -25846,7 +25852,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="131" spans="1:128" s="9" customFormat="1">
+    <row r="131" spans="1:128" s="9" customFormat="1" ht="409.6">
       <c r="A131" s="7" t="s">
         <v>399</v>
       </c>
@@ -26473,7 +26479,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="135" spans="1:128" s="9" customFormat="1">
+    <row r="135" spans="1:128" s="9" customFormat="1" ht="409.6">
       <c r="A135" s="7" t="s">
         <v>400</v>
       </c>
@@ -27119,7 +27125,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="139" spans="1:128" s="9" customFormat="1">
+    <row r="139" spans="1:128" s="9" customFormat="1" ht="409.6">
       <c r="A139" s="7" t="s">
         <v>401</v>
       </c>
@@ -27745,7 +27751,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="143" spans="1:128" s="9" customFormat="1">
+    <row r="143" spans="1:128" s="9" customFormat="1" ht="409.6">
       <c r="A143" s="7" t="s">
         <v>402</v>
       </c>
@@ -28391,7 +28397,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="147" spans="1:129" s="9" customFormat="1">
+    <row r="147" spans="1:129" s="9" customFormat="1" ht="409.6">
       <c r="A147" s="7" t="s">
         <v>403</v>
       </c>
@@ -28896,7 +28902,7 @@
         <v>3</v>
       </c>
       <c r="X149" s="14" t="s">
-        <v>317</v>
+        <v>431</v>
       </c>
       <c r="Y149" s="5" t="s">
         <v>14</v>
@@ -29048,7 +29054,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="151" spans="1:129" s="32" customFormat="1">
+    <row r="151" spans="1:129" s="32" customFormat="1" ht="409.6">
       <c r="A151" s="29"/>
       <c r="B151" s="30"/>
       <c r="C151" s="29"/>
@@ -29152,10 +29158,10 @@
       <c r="CY151" s="31"/>
       <c r="CZ151" s="31"/>
     </row>
-    <row r="152" spans="1:129">
+    <row r="152" spans="1:129" ht="409.6">
       <c r="A152" s="52"/>
     </row>
-    <row r="153" spans="1:129" s="32" customFormat="1">
+    <row r="153" spans="1:129" s="32" customFormat="1" ht="409.6">
       <c r="A153" s="29"/>
       <c r="B153" s="30"/>
       <c r="C153" s="29"/>
@@ -29259,7 +29265,7 @@
       <c r="CY153" s="31"/>
       <c r="CZ153" s="31"/>
     </row>
-    <row r="154" spans="1:129" s="25" customFormat="1">
+    <row r="154" spans="1:129" s="25" customFormat="1" ht="409.6">
       <c r="A154" s="7" t="s">
         <v>214</v>
       </c>

</xml_diff>